<commit_message>
ASK-41 Also read common sections again
</commit_message>
<xml_diff>
--- a/benchmarktests/assembly.kernel.benchmark.tests.io.tests/test-data/Benchmarktool Excel assemblagetool - General information.xlsx
+++ b/benchmarktests/assembly.kernel.benchmark.tests.io.tests/test-data/Benchmarktool Excel assemblagetool - General information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\wbi-assemblage-rekenkern\benchmarktests\assembly.kernel.benchmark.tests.io.tests\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92FD590-F3B3-4587-8970-1C95B7AFDC42}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE5F746-C144-42BE-A8C1-4BDC4ED6E580}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="7800" windowWidth="28800" windowHeight="15435" tabRatio="653" xr2:uid="{34AC3CB5-6C6A-4A77-BC52-5E824B97181F}"/>
+    <workbookView xWindow="-28800" yWindow="7950" windowWidth="28800" windowHeight="15435" tabRatio="653" xr2:uid="{34AC3CB5-6C6A-4A77-BC52-5E824B97181F}"/>
   </bookViews>
   <sheets>
     <sheet name="Normen en duidingsklassen" sheetId="13" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Signaleringskans</t>
   </si>
@@ -76,9 +76,6 @@
   </si>
   <si>
     <t>+0</t>
-  </si>
-  <si>
-    <t>0</t>
   </si>
   <si>
     <t>-I</t>
@@ -126,7 +123,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,12 +174,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -323,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -343,10 +334,9 @@
     <xf numFmtId="49" fontId="0" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="11" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -689,7 +679,7 @@
   <dimension ref="A2:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,7 +694,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>9</v>
@@ -736,7 +726,7 @@
         <f>1/1000</f>
         <v>1E-3</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="23" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="3">
@@ -749,12 +739,12 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>10.4</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="24" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="4">
@@ -767,7 +757,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="25" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="4">
@@ -780,7 +770,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="26" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="4">
@@ -793,7 +783,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="27" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="6">
@@ -806,12 +796,12 @@
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D12" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" s="14" t="s">
         <v>8</v>
@@ -822,8 +812,8 @@
         <v>11</v>
       </c>
       <c r="E13" s="9">
-        <f>1/30*B3</f>
-        <v>1.111111111111111E-5</v>
+        <f>1/1000*B3</f>
+        <v>3.3333333333333335E-7</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -831,8 +821,8 @@
         <v>12</v>
       </c>
       <c r="E14" s="9">
-        <f>1/10*B3</f>
-        <v>3.3333333333333335E-5</v>
+        <f>1/100*B3</f>
+        <v>3.3333333333333333E-6</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -840,8 +830,8 @@
         <v>13</v>
       </c>
       <c r="E15" s="9">
-        <f>1/3*B3</f>
-        <v>1.111111111111111E-4</v>
+        <f>1/10*B3</f>
+        <v>3.3333333333333335E-5</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -867,38 +857,32 @@
         <v>16</v>
       </c>
       <c r="E18" s="9">
-        <f>3*B4</f>
-        <v>3.0000000000000001E-3</v>
+        <f>10*B4</f>
+        <v>0.01</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D19" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="9">
-        <f>10*B4</f>
-        <v>0.01</v>
+      <c r="E19" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D20" s="22" t="s">
+      <c r="D20" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D21" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D22" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="7"/>
+      <c r="E21" s="7"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D22" s="11"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D23" s="11"/>

</xml_diff>